<commit_message>
Adding RES to notebook
* Added model's simplified RES to notebook to aid with exercises
</commit_message>
<xml_diff>
--- a/Book_Exercise_Files/Demand_Profile_Samples.xlsx
+++ b/Book_Exercise_Files/Demand_Profile_Samples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/940a138d5667ee1b/Documentos/UVic/Courses/UVIC-2023/Spring-2023/IESVic-Coop/Storage-Master/Wiki/IESVic_OSeMOSYS_Book/Book_Exercise_Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/940a138d5667ee1b/Documentos/UVic/Courses/UVIC-2023/Spring-2023/IESVic-Coop/The_OSeMOSYS_EBook_by_IESVic/Book_Exercise_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="171" documentId="11_F25DC773A252ABDACC104806A19B57945ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F378657A-C3EA-4D3B-935F-31C9E8080204}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="11_F25DC773A252ABDACC104806A19B57945ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFDA9A11-67B0-40EB-8FC9-C13B598D7A12}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SDP_Sample1" sheetId="1" r:id="rId1"/>
@@ -115,10 +115,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
-    <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -198,29 +195,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -326,310 +300,16 @@
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -642,10 +322,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -665,7 +341,7 @@
     <tableColumn id="5" xr3:uid="{117360E2-5728-44D2-8A5D-E1C4228CA1CE}" name="Year">
       <calculatedColumnFormula>E1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7A5F4E7B-5EE1-4EDE-86A6-9F20B80309A9}" name="Specified_Demand_Profile" dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{7A5F4E7B-5EE1-4EDE-86A6-9F20B80309A9}" name="Specified_Demand_Profile" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -688,7 +364,7 @@
     <tableColumn id="5" xr3:uid="{357D283D-7260-4180-84A3-0D288DC1469A}" name="Year">
       <calculatedColumnFormula>E1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5443AF3E-6CEC-4072-9E09-ABE389F89399}" name="Specified_Demand_Profile" dataDxfId="33">
+    <tableColumn id="6" xr3:uid="{5443AF3E-6CEC-4072-9E09-ABE389F89399}" name="Specified_Demand_Profile" dataDxfId="21">
       <calculatedColumnFormula>1/48</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -716,7 +392,7 @@
     <tableColumn id="5" xr3:uid="{641B8ABD-EA9D-4486-82AB-009A43FBA255}" name="Year">
       <calculatedColumnFormula>E1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9A79A3D0-109A-41D0-8D6B-48B10881936E}" name="Specified_Demand_Profile" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{9A79A3D0-109A-41D0-8D6B-48B10881936E}" name="Specified_Demand_Profile" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -739,7 +415,7 @@
     <tableColumn id="5" xr3:uid="{CF4850CC-4492-456A-8BB5-FFE7540C1B3E}" name="Year">
       <calculatedColumnFormula>E1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7122F1F9-8B88-4AAC-8CF3-76DC8D12D497}" name="Specified_Demand_Profile" dataDxfId="11">
+    <tableColumn id="6" xr3:uid="{7122F1F9-8B88-4AAC-8CF3-76DC8D12D497}" name="Specified_Demand_Profile" dataDxfId="19">
       <calculatedColumnFormula>1/50</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -764,7 +440,7 @@
     <tableColumn id="5" xr3:uid="{3DF4C63B-CFBA-49A6-92A9-27F49B4DDEC1}" name="Year">
       <calculatedColumnFormula>E1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A93A25D1-5798-4679-A661-BB56447C2D16}" name="Specified_Demand_Profile" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{A93A25D1-5798-4679-A661-BB56447C2D16}" name="Specified_Demand_Profile" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1035,11 +711,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection sqref="A1:F49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="25.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2211,42 +1890,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F1 A2:E49">
-    <cfRule type="cellIs" dxfId="54" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F14:F48">
-    <cfRule type="cellIs" dxfId="52" priority="7" operator="equal">
+  <conditionalFormatting sqref="F2:F49">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="8" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F25">
-    <cfRule type="cellIs" dxfId="50" priority="5" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="6" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26:F48">
-    <cfRule type="cellIs" dxfId="48" priority="3" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F49">
-    <cfRule type="cellIs" dxfId="46" priority="1" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3488,42 +3143,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F1 A2:E49">
-    <cfRule type="cellIs" dxfId="43" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F14:F48">
-    <cfRule type="cellIs" dxfId="41" priority="7" operator="equal">
+  <conditionalFormatting sqref="F2:F49">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="8" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F25">
-    <cfRule type="cellIs" dxfId="39" priority="5" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="6" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26:F48">
-    <cfRule type="cellIs" dxfId="37" priority="3" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F49">
-    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4621,42 +4252,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F1 A2:E49">
-    <cfRule type="cellIs" dxfId="32" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F14:F48">
-    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
+  <conditionalFormatting sqref="F2:F49">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F25">
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26:F48">
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F49">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5898,42 +5505,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F1 A2:E49">
-    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F14:F48">
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+  <conditionalFormatting sqref="F2:F49">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F27">
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26:F48">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F49">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5948,7 +5531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{305444A6-D613-4023-9844-18919AFE5866}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -7127,10 +6710,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F1 A2:E49">
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>